<commit_message>
updated translation evaluation results
</commit_message>
<xml_diff>
--- a/translation_stats/codellama_avatar_compileReport_from_java_to_python_misleading_test.xlsx
+++ b/translation_stats/codellama_avatar_compileReport_from_java_to_python_misleading_test.xlsx
@@ -596,7 +596,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>codeforces_334_A.py</t>
+          <t>atcoder_ABC169_C.py</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>atcoder_ABC169_C.py</t>
+          <t>atcoder_ABC174_C.py</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>codeforces_189_A.py</t>
+          <t>atcoder_ABC051_A.py</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>atcoder_ABC174_C.py</t>
+          <t>atcoder_ABC132_F.py</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>atcoder_ABC132_F.py</t>
+          <t>codeforces_334_A.py</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>codeforces_306_A.py</t>
+          <t>codeforces_189_A.py</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>atcoder_ABC051_A.py</t>
+          <t>atcoder_ABC124_C.py</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>atcoder_ABC124_C.py</t>
+          <t>codeforces_96_B.py</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>codeforces_96_B.py</t>
+          <t>codeforces_306_A.py</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>codeforces_110_B.py</t>
+          <t>atcoder_ABC122_D.py</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>atcoder_ARC062_B.py</t>
+          <t>atcoder_ABC108_B.py</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>atcoder_ABC136_B.py</t>
+          <t>codeforces_651_A.py</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>atcoder_ABC125_A.py</t>
+          <t>codeforces_171_A.py</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>atcoder_ABC172_D.py</t>
+          <t>atcoder_AGC046_A.py</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -971,7 +971,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>atcoder_ABC114_C.py</t>
+          <t>atcoder_ARC102_C.py</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>codeforces_514_A.py</t>
+          <t>codeforces_276_B.py</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>atcoder_AGC002_A.py</t>
+          <t>codeforces_86_A.py</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>codeforces_58_B.py</t>
+          <t>codeforces_544_B.py</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>codeforces_622_A.py</t>
+          <t>atcoder_ABC042_A.py</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1096,12 +1096,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>codeforces_669_A.py</t>
+          <t>atcoder_ABC136_B.py</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Infinite Loop</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1121,12 +1121,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>codeforces_340_A.py</t>
+          <t>codeforces_581_A.py</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Infinite Loop</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1146,12 +1146,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>atcoder_AGC046_A.py</t>
+          <t>codeforces_242_A.py</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1171,12 +1171,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>atcoder_ABC043_B.py</t>
+          <t>codeforces_569_A.py</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1196,12 +1196,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>codeforces_147_A.py</t>
+          <t>atcoder_ABC070_B.py</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1221,12 +1221,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>atcoder_ABC169_D.py</t>
+          <t>codeforces_672_A.py</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1246,12 +1246,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>atcoder_ABC108_B.py</t>
+          <t>codeforces_55_A.py</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>codeforces_59_A.py</t>
+          <t>atcoder_ABC043_B.py</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1321,12 +1321,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>codeforces_276_B.py</t>
+          <t>codeforces_678_B.py</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1346,12 +1346,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>codeforces_546_A.py</t>
+          <t>atcoder_ABC120_C.py</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1371,12 +1371,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>atcoder_ABC143_A.py</t>
+          <t>codeforces_379_A.py</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>atcoder_ABC132_A.py</t>
+          <t>codeforces_79_A.py</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1421,12 +1421,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>codeforces_242_A.py</t>
+          <t>atcoder_ABC143_A.py</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1446,12 +1446,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>atcoder_ABC122_D.py</t>
+          <t>atcoder_ABC153_A.py</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1471,12 +1471,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>codeforces_369_B.py</t>
+          <t>codeforces_110_B.py</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1496,12 +1496,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>codeforces_49_A.py</t>
+          <t>codeforces_459_A.py</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1521,12 +1521,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>atcoder_ABC124_A.py</t>
+          <t>atcoder_ABC178_B.py</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1546,12 +1546,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>atcoder_ABC070_B.py</t>
+          <t>atcoder_AGC046_B.py</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1571,12 +1571,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>atcoder_ABC155_E.py</t>
+          <t>atcoder_ABC172_D.py</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1596,12 +1596,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>codeforces_678_B.py</t>
+          <t>codeforces_369_B.py</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1621,12 +1621,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>codeforces_55_A.py</t>
+          <t>codeforces_546_A.py</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1646,12 +1646,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>atcoder_ABC170_A.py</t>
+          <t>atcoder_ABC149_B.py</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1671,12 +1671,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>atcoder_ARC102_C.py</t>
+          <t>atcoder_ABC151_A.py</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1696,12 +1696,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>atcoder_ABC151_A.py</t>
+          <t>atcoder_ABC168_C.py</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1721,12 +1721,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>codeforces_8_B.py</t>
+          <t>codeforces_58_B.py</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1746,12 +1746,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>codeforces_190_A.py</t>
+          <t>atcoder_ABC132_A.py</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1771,12 +1771,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>codeforces_672_A.py</t>
+          <t>codeforces_99_A.py</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1796,12 +1796,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>atcoder_AGC046_B.py</t>
+          <t>codeforces_514_A.py</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1821,12 +1821,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>atcoder_ABC168_C.py</t>
+          <t>codeforces_8_B.py</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1846,12 +1846,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>codeforces_79_A.py</t>
+          <t>atcoder_ABC127_B.py</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1871,12 +1871,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>codeforces_86_A.py</t>
+          <t>atcoder_ABC158_B.py</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1896,12 +1896,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>codeforces_30_A.py</t>
+          <t>codeforces_92_A.py</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1921,12 +1921,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>codeforces_459_A.py</t>
+          <t>atcoder_ABC124_A.py</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1946,12 +1946,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>atcoder_ABC149_B.py</t>
+          <t>codeforces_59_A.py</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -1971,12 +1971,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>codeforces_544_B.py</t>
+          <t>codeforces_49_A.py</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2021,12 +2021,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>codeforces_581_A.py</t>
+          <t>atcoder_ABC139_B.py</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2046,12 +2046,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>codeforces_99_A.py</t>
+          <t>codeforces_30_A.py</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2071,12 +2071,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>codeforces_32_B.py</t>
+          <t>codeforces_622_A.py</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2096,12 +2096,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>codeforces_379_A.py</t>
+          <t>atcoder_ABC164_A.py</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2121,12 +2121,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>atcoder_ABC158_A.py</t>
+          <t>atcoder_AGC002_A.py</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2146,12 +2146,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>codeforces_171_A.py</t>
+          <t>atcoder_ABC158_A.py</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2171,12 +2171,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>atcoder_ABC158_B.py</t>
+          <t>atcoder_ARC062_B.py</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2196,12 +2196,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>atcoder_ABC042_A.py</t>
+          <t>atcoder_ABC155_E.py</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2221,12 +2221,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>atcoder_ABC178_B.py</t>
+          <t>atcoder_ABC142_A.py</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2246,12 +2246,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>codeforces_569_A.py</t>
+          <t>atcoder_ABC170_A.py</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2271,12 +2271,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>atcoder_ABC164_A.py</t>
+          <t>codeforces_190_A.py</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2296,12 +2296,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>atcoder_AGC006_B.py</t>
+          <t>atcoder_ABC114_C.py</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2321,12 +2321,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>atcoder_ABC120_C.py</t>
+          <t>atcoder_ABC125_A.py</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2346,12 +2346,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>codeforces_92_A.py</t>
+          <t>atcoder_ABC169_D.py</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2371,12 +2371,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>atcoder_ABC127_B.py</t>
+          <t>codeforces_32_B.py</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Test Failed</t>
         </is>
       </c>
     </row>
@@ -2396,12 +2396,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>atcoder_ABC153_A.py</t>
+          <t>codeforces_669_A.py</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Infinite Loop</t>
         </is>
       </c>
     </row>
@@ -2421,12 +2421,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>atcoder_ABC139_B.py</t>
+          <t>codeforces_340_A.py</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Correct</t>
+          <t>Infinite Loop</t>
         </is>
       </c>
     </row>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>atcoder_ABC142_A.py</t>
+          <t>codeforces_147_A.py</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>codeforces_651_A.py</t>
+          <t>atcoder_AGC006_B.py</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">

</xml_diff>